<commit_message>
correções DDL e Dicionário de Dados
</commit_message>
<xml_diff>
--- a/Banco de Dados/Dicionário_de_Dados.xlsx
+++ b/Banco de Dados/Dicionário_de_Dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thaysa\Documents\4ºSemestre\InterDisiplinar\FloatGroup\FloatGroup\Banco de Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gui\Documents\FloatGroup\FloatGroup\Banco de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="87">
   <si>
     <t>Tabela</t>
   </si>
@@ -279,13 +279,19 @@
   </si>
   <si>
     <t>periodo</t>
+  </si>
+  <si>
+    <t>blob</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +300,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -347,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -381,21 +394,23 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -694,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F148" sqref="F148:F149"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,34 +722,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -877,34 +892,34 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -992,8 +1007,8 @@
       <c r="E14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>20</v>
+      <c r="F14" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>19</v>
@@ -1117,34 +1132,34 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="A20" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1701,34 +1716,34 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="4" t="s">
+      <c r="A40" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
@@ -1836,34 +1851,34 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="4" t="s">
+      <c r="A47" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
@@ -1951,8 +1966,8 @@
       <c r="E51" s="3">
         <v>2</v>
       </c>
-      <c r="F51" s="8" t="s">
-        <v>20</v>
+      <c r="F51" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>19</v>
@@ -1986,8 +2001,8 @@
       <c r="E52" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F52" s="8" t="s">
-        <v>20</v>
+      <c r="F52" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>19</v>
@@ -2006,34 +2021,34 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="4" t="s">
+      <c r="A55" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
@@ -2140,127 +2155,127 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B62" s="4" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C60" s="4">
+        <v>5</v>
+      </c>
+      <c r="D60" s="4">
+        <v>10</v>
+      </c>
+      <c r="E60" s="4">
+        <v>2</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="13"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E64" s="3" t="s">
+      <c r="D65" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F65" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G65" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H65" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I64" s="3" t="s">
+      <c r="I65" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J64" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K64" s="3" t="s">
+      <c r="J65" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K65" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C65" s="7">
-        <v>4</v>
-      </c>
-      <c r="D65" s="7">
-        <v>10</v>
-      </c>
-      <c r="E65" s="7">
-        <v>0</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G65" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H65" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I65" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K65" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C66" s="7">
-        <v>100</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>18</v>
+        <v>4</v>
+      </c>
+      <c r="D66" s="7">
+        <v>10</v>
+      </c>
+      <c r="E66" s="7">
+        <v>0</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>19</v>
@@ -2277,13 +2292,13 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C67" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>18</v>
@@ -2292,7 +2307,7 @@
         <v>18</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>19</v>
@@ -2312,7 +2327,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>16</v>
@@ -2347,7 +2362,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>16</v>
@@ -2382,7 +2397,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>16</v>
@@ -2415,171 +2430,171 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" s="4" t="s">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" s="7">
+        <v>50</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="4"/>
-      <c r="K74" s="4"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="13"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E75" s="3" t="s">
+      <c r="D76" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="F76" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G75" s="3" t="s">
+      <c r="G76" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H75" s="3" t="s">
+      <c r="H76" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I75" s="3" t="s">
+      <c r="I76" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J75" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K75" s="3" t="s">
+      <c r="J76" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K76" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B77" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C76" s="7">
-        <v>4</v>
-      </c>
-      <c r="D76" s="7">
-        <v>10</v>
-      </c>
-      <c r="E76" s="7">
-        <v>0</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G76" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H76" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I76" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J76" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K76" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
+      <c r="C77" s="7">
+        <v>4</v>
+      </c>
+      <c r="D77" s="7">
+        <v>10</v>
+      </c>
+      <c r="E77" s="7">
+        <v>0</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K77" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C77" s="3">
-        <v>4</v>
-      </c>
-      <c r="D77" s="3">
-        <v>10</v>
-      </c>
-      <c r="E77" s="3">
-        <v>0</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G77" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I77" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J77" s="3" t="s">
+      <c r="C78" s="3">
+        <v>4</v>
+      </c>
+      <c r="D78" s="3">
+        <v>10</v>
+      </c>
+      <c r="E78" s="3">
+        <v>0</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G78" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J78" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="K77" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C78" s="7">
-        <v>50</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G78" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H78" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I78" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J78" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="K78" s="3" t="s">
         <v>18</v>
@@ -2587,190 +2602,194 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" s="7">
+        <v>50</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I79" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J79" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K79" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
-      <c r="F79" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G79" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H79" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I79" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J79" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K79" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B82" s="4" t="s">
+      <c r="B80" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G80" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H80" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I80" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J80" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K80" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="4"/>
-      <c r="K82" s="4"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
-      <c r="H83" s="4"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="4"/>
-      <c r="K83" s="4"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13"/>
+      <c r="K83" s="13"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="13"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="13"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C85" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E84" s="3" t="s">
+      <c r="D85" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F84" s="3" t="s">
+      <c r="F85" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G84" s="3" t="s">
+      <c r="G85" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H84" s="3" t="s">
+      <c r="H85" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I84" s="3" t="s">
+      <c r="I85" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J84" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K84" s="3" t="s">
+      <c r="J85" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K85" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="B86" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C85" s="7">
-        <v>4</v>
-      </c>
-      <c r="D85" s="7">
-        <v>10</v>
-      </c>
-      <c r="E85" s="7">
-        <v>0</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H85" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I85" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J85" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K85" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
+      <c r="C86" s="7">
+        <v>4</v>
+      </c>
+      <c r="D86" s="7">
+        <v>10</v>
+      </c>
+      <c r="E86" s="7">
+        <v>0</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H86" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I86" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B87" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G86" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J86" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K86" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C87" s="7">
-        <v>4</v>
-      </c>
-      <c r="D87" s="3">
-        <v>10</v>
-      </c>
-      <c r="E87" s="3">
-        <v>0</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G87" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H87" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I87" s="7" t="s">
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G87" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I87" s="3" t="s">
         <v>19</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="K87" s="3" t="s">
         <v>18</v>
@@ -2778,7 +2797,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>15</v>
@@ -2792,433 +2811,433 @@
       <c r="E88" s="3">
         <v>0</v>
       </c>
-      <c r="F88" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G88" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H88" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I88" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J88" s="10" t="s">
+      <c r="F88" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G88" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H88" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I88" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="7">
+        <v>4</v>
+      </c>
+      <c r="D89" s="3">
+        <v>10</v>
+      </c>
+      <c r="E89" s="3">
+        <v>0</v>
+      </c>
+      <c r="F89" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G89" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H89" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I89" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J89" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K88" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B91" s="4" t="s">
+      <c r="K89" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
-      <c r="G91" s="4"/>
-      <c r="H91" s="4"/>
-      <c r="I91" s="4"/>
-      <c r="J91" s="4"/>
-      <c r="K91" s="4"/>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
-      <c r="G92" s="4"/>
-      <c r="H92" s="4"/>
-      <c r="I92" s="4"/>
-      <c r="J92" s="4"/>
-      <c r="K92" s="4"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="13"/>
+      <c r="K92" s="13"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="13"/>
+      <c r="B93" s="13"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
+      <c r="G93" s="13"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="13"/>
+      <c r="K93" s="13"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B94" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C94" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E93" s="3" t="s">
+      <c r="D94" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E94" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F93" s="3" t="s">
+      <c r="F94" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G93" s="3" t="s">
+      <c r="G94" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H93" s="3" t="s">
+      <c r="H94" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I93" s="3" t="s">
+      <c r="I94" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J93" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K93" s="3" t="s">
+      <c r="J94" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K94" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="B95" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C94" s="7">
-        <v>4</v>
-      </c>
-      <c r="D94" s="7">
-        <v>10</v>
-      </c>
-      <c r="E94" s="7">
-        <v>0</v>
-      </c>
-      <c r="F94" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G94" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H94" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I94" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J94" s="3" t="s">
+      <c r="C95" s="7">
+        <v>4</v>
+      </c>
+      <c r="D95" s="7">
+        <v>10</v>
+      </c>
+      <c r="E95" s="7">
+        <v>0</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H95" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I95" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J95" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K94" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
+      <c r="K95" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B96" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C95" s="3">
-        <v>4</v>
-      </c>
-      <c r="D95" s="3">
-        <v>10</v>
-      </c>
-      <c r="E95" s="3">
-        <v>0</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G95" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I95" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J95" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K95" s="3" t="s">
+      <c r="C96" s="3">
+        <v>4</v>
+      </c>
+      <c r="D96" s="3">
+        <v>10</v>
+      </c>
+      <c r="E96" s="3">
+        <v>0</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J96" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K96" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B96" s="7" t="s">
+      <c r="B97" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C96" s="7">
+      <c r="C97" s="7">
         <v>5</v>
       </c>
-      <c r="D96" s="3">
+      <c r="D97" s="3">
         <v>15</v>
       </c>
-      <c r="E96" s="3">
+      <c r="E97" s="3">
         <v>2</v>
       </c>
-      <c r="F96" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G96" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H96" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I96" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J96" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K96" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B99" s="4" t="s">
+      <c r="F97" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G97" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H97" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I97" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J97" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K97" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C99" s="4"/>
-      <c r="D99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4"/>
-      <c r="G99" s="4"/>
-      <c r="H99" s="4"/>
-      <c r="I99" s="4"/>
-      <c r="J99" s="4"/>
-      <c r="K99" s="4"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4"/>
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
-      <c r="I100" s="4"/>
-      <c r="J100" s="4"/>
-      <c r="K100" s="4"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="13"/>
+      <c r="K100" s="13"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="13"/>
+      <c r="B101" s="13"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="13"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="13"/>
+      <c r="K101" s="13"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B102" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C102" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E101" s="3" t="s">
+      <c r="D102" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E102" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F101" s="3" t="s">
+      <c r="F102" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G101" s="3" t="s">
+      <c r="G102" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H101" s="3" t="s">
+      <c r="H102" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I101" s="3" t="s">
+      <c r="I102" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J101" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K101" s="3" t="s">
+      <c r="J102" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K102" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="B103" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C102" s="7">
-        <v>4</v>
-      </c>
-      <c r="D102" s="7">
-        <v>10</v>
-      </c>
-      <c r="E102" s="7">
-        <v>0</v>
-      </c>
-      <c r="F102" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G102" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H102" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I102" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J102" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K102" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
+      <c r="C103" s="7">
+        <v>4</v>
+      </c>
+      <c r="D103" s="7">
+        <v>10</v>
+      </c>
+      <c r="E103" s="7">
+        <v>0</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G103" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H103" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I103" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J103" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B104" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C103" s="3">
+      <c r="C104" s="3">
         <v>80</v>
       </c>
-      <c r="D103" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F103" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G103" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H103" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I103" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J103" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K103" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B106" s="4" t="s">
+      <c r="D104" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F104" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G104" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J104" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="4"/>
-      <c r="G106" s="4"/>
-      <c r="H106" s="4"/>
-      <c r="I106" s="4"/>
-      <c r="J106" s="4"/>
-      <c r="K106" s="4"/>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
-      <c r="H107" s="4"/>
-      <c r="I107" s="4"/>
-      <c r="J107" s="4"/>
-      <c r="K107" s="4"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="13"/>
+      <c r="J107" s="13"/>
+      <c r="K107" s="13"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="13"/>
+      <c r="B108" s="13"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="13"/>
+      <c r="H108" s="13"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="13"/>
+      <c r="K108" s="13"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B109" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E108" s="3" t="s">
+      <c r="D109" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E109" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F108" s="3" t="s">
+      <c r="F109" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G108" s="3" t="s">
+      <c r="G109" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H108" s="3" t="s">
+      <c r="H109" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I108" s="3" t="s">
+      <c r="I109" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J108" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K108" s="3" t="s">
+      <c r="J109" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K109" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B109" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C109" s="7">
-        <v>4</v>
-      </c>
-      <c r="D109" s="7">
-        <v>10</v>
-      </c>
-      <c r="E109" s="7">
-        <v>0</v>
-      </c>
-      <c r="F109" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G109" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H109" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I109" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J109" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K109" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B110" s="7" t="s">
         <v>15</v>
@@ -3226,10 +3245,10 @@
       <c r="C110" s="7">
         <v>4</v>
       </c>
-      <c r="D110" s="3">
-        <v>10</v>
-      </c>
-      <c r="E110" s="3">
+      <c r="D110" s="7">
+        <v>10</v>
+      </c>
+      <c r="E110" s="7">
         <v>0</v>
       </c>
       <c r="F110" s="7" t="s">
@@ -3245,7 +3264,7 @@
         <v>19</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K110" s="3" t="s">
         <v>18</v>
@@ -3253,7 +3272,7 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>15</v>
@@ -3271,16 +3290,16 @@
         <v>19</v>
       </c>
       <c r="G111" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H111" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I111" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J111" s="3" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="K111" s="3" t="s">
         <v>18</v>
@@ -3288,22 +3307,22 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C112" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D112" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E112" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G112" s="7" t="s">
         <v>19</v>
@@ -3323,154 +3342,160 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C113" s="7">
+        <v>5</v>
+      </c>
+      <c r="D113" s="3">
+        <v>15</v>
+      </c>
+      <c r="E113" s="3">
+        <v>2</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G113" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H113" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I113" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J113" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K113" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B113" s="7" t="s">
+      <c r="B114" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C113" s="7">
-        <v>4</v>
-      </c>
-      <c r="D113" s="3">
-        <v>10</v>
-      </c>
-      <c r="E113" s="3">
-        <v>0</v>
-      </c>
-      <c r="F113" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G113" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H113" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I113" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J113" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K113" s="3" t="s">
+      <c r="C114" s="7">
+        <v>4</v>
+      </c>
+      <c r="D114" s="3">
+        <v>10</v>
+      </c>
+      <c r="E114" s="3">
+        <v>0</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G114" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H114" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I114" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K114" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B116" s="4" t="s">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C116" s="4"/>
-      <c r="D116" s="4"/>
-      <c r="E116" s="4"/>
-      <c r="F116" s="4"/>
-      <c r="G116" s="4"/>
-      <c r="H116" s="4"/>
-      <c r="I116" s="4"/>
-      <c r="J116" s="4"/>
-      <c r="K116" s="4"/>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="4"/>
-      <c r="B117" s="4"/>
-      <c r="C117" s="4"/>
-      <c r="D117" s="4"/>
-      <c r="E117" s="4"/>
-      <c r="F117" s="4"/>
-      <c r="G117" s="4"/>
-      <c r="H117" s="4"/>
-      <c r="I117" s="4"/>
-      <c r="J117" s="4"/>
-      <c r="K117" s="4"/>
+      <c r="C117" s="13"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="13"/>
+      <c r="F117" s="13"/>
+      <c r="G117" s="13"/>
+      <c r="H117" s="13"/>
+      <c r="I117" s="13"/>
+      <c r="J117" s="13"/>
+      <c r="K117" s="13"/>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
+      <c r="A118" s="13"/>
+      <c r="B118" s="13"/>
+      <c r="C118" s="13"/>
+      <c r="D118" s="13"/>
+      <c r="E118" s="13"/>
+      <c r="F118" s="13"/>
+      <c r="G118" s="13"/>
+      <c r="H118" s="13"/>
+      <c r="I118" s="13"/>
+      <c r="J118" s="13"/>
+      <c r="K118" s="13"/>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B119" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D118" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E118" s="3" t="s">
+      <c r="D119" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E119" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F118" s="3" t="s">
+      <c r="F119" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G118" s="3" t="s">
+      <c r="G119" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H118" s="3" t="s">
+      <c r="H119" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I118" s="3" t="s">
+      <c r="I119" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J118" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K118" s="3" t="s">
+      <c r="J119" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K119" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C119" s="7">
-        <v>4</v>
-      </c>
-      <c r="D119" s="7">
-        <v>10</v>
-      </c>
-      <c r="E119" s="7">
-        <v>0</v>
-      </c>
-      <c r="F119" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G119" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H119" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I119" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J119" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K119" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B120" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C120" s="11"/>
-      <c r="D120" s="8"/>
-      <c r="E120" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C120" s="7">
+        <v>4</v>
+      </c>
+      <c r="D120" s="7">
+        <v>10</v>
+      </c>
+      <c r="E120" s="7">
+        <v>0</v>
+      </c>
       <c r="F120" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G120" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H120" s="7" t="s">
         <v>19</v>
@@ -3487,20 +3512,14 @@
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B121" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C121" s="7">
-        <v>4</v>
-      </c>
-      <c r="D121" s="3">
-        <v>10</v>
-      </c>
-      <c r="E121" s="3">
-        <v>0</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B121" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C121" s="11"/>
+      <c r="D121" s="8"/>
+      <c r="E121" s="8"/>
       <c r="F121" s="7" t="s">
         <v>19</v>
       </c>
@@ -3517,12 +3536,12 @@
         <v>18</v>
       </c>
       <c r="K121" s="3" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>15</v>
@@ -3543,21 +3562,21 @@
         <v>19</v>
       </c>
       <c r="H122" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I122" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J122" s="3" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="K122" s="3" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B123" s="7" t="s">
         <v>15</v>
@@ -3565,10 +3584,10 @@
       <c r="C123" s="7">
         <v>4</v>
       </c>
-      <c r="D123" s="7">
-        <v>10</v>
-      </c>
-      <c r="E123" s="7">
+      <c r="D123" s="3">
+        <v>10</v>
+      </c>
+      <c r="E123" s="3">
         <v>0</v>
       </c>
       <c r="F123" s="7" t="s">
@@ -3584,115 +3603,115 @@
         <v>19</v>
       </c>
       <c r="J123" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K123" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C124" s="7">
+        <v>4</v>
+      </c>
+      <c r="D124" s="7">
+        <v>10</v>
+      </c>
+      <c r="E124" s="7">
+        <v>0</v>
+      </c>
+      <c r="F124" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G124" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H124" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I124" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J124" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K123" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A126" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B126" s="4" t="s">
+      <c r="K124" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C126" s="4"/>
-      <c r="D126" s="4"/>
-      <c r="E126" s="4"/>
-      <c r="F126" s="4"/>
-      <c r="G126" s="4"/>
-      <c r="H126" s="4"/>
-      <c r="I126" s="4"/>
-      <c r="J126" s="4"/>
-      <c r="K126" s="4"/>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A127" s="4"/>
-      <c r="B127" s="4"/>
-      <c r="C127" s="4"/>
-      <c r="D127" s="4"/>
-      <c r="E127" s="4"/>
-      <c r="F127" s="4"/>
-      <c r="G127" s="4"/>
-      <c r="H127" s="4"/>
-      <c r="I127" s="4"/>
-      <c r="J127" s="4"/>
-      <c r="K127" s="4"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="13"/>
+      <c r="F127" s="13"/>
+      <c r="G127" s="13"/>
+      <c r="H127" s="13"/>
+      <c r="I127" s="13"/>
+      <c r="J127" s="13"/>
+      <c r="K127" s="13"/>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="13"/>
+      <c r="B128" s="13"/>
+      <c r="C128" s="13"/>
+      <c r="D128" s="13"/>
+      <c r="E128" s="13"/>
+      <c r="F128" s="13"/>
+      <c r="G128" s="13"/>
+      <c r="H128" s="13"/>
+      <c r="I128" s="13"/>
+      <c r="J128" s="13"/>
+      <c r="K128" s="13"/>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B129" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C128" s="3" t="s">
+      <c r="C129" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D128" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E128" s="3" t="s">
+      <c r="D129" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E129" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F128" s="3" t="s">
+      <c r="F129" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G128" s="3" t="s">
+      <c r="G129" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H128" s="3" t="s">
+      <c r="H129" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I128" s="3" t="s">
+      <c r="I129" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J128" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K128" s="3" t="s">
+      <c r="J129" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K129" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B129" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C129" s="7">
-        <v>4</v>
-      </c>
-      <c r="D129" s="7">
-        <v>10</v>
-      </c>
-      <c r="E129" s="7">
-        <v>0</v>
-      </c>
-      <c r="F129" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G129" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H129" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I129" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J129" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="K129" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B130" s="7" t="s">
         <v>15</v>
@@ -3700,10 +3719,10 @@
       <c r="C130" s="7">
         <v>4</v>
       </c>
-      <c r="D130" s="3">
-        <v>10</v>
-      </c>
-      <c r="E130" s="3">
+      <c r="D130" s="7">
+        <v>10</v>
+      </c>
+      <c r="E130" s="7">
         <v>0</v>
       </c>
       <c r="F130" s="7" t="s">
@@ -3719,7 +3738,7 @@
         <v>19</v>
       </c>
       <c r="J130" s="3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="K130" s="3" t="s">
         <v>18</v>
@@ -3727,7 +3746,7 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B131" s="7" t="s">
         <v>15</v>
@@ -3745,142 +3764,142 @@
         <v>19</v>
       </c>
       <c r="G131" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I131" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J131" s="3" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="K131" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A134" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B134" s="4" t="s">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C132" s="7">
+        <v>4</v>
+      </c>
+      <c r="D132" s="3">
+        <v>10</v>
+      </c>
+      <c r="E132" s="3">
+        <v>0</v>
+      </c>
+      <c r="F132" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G132" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H132" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I132" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J132" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K132" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A135" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B135" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C134" s="4"/>
-      <c r="D134" s="4"/>
-      <c r="E134" s="4"/>
-      <c r="F134" s="4"/>
-      <c r="G134" s="4"/>
-      <c r="H134" s="4"/>
-      <c r="I134" s="4"/>
-      <c r="J134" s="4"/>
-      <c r="K134" s="4"/>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135" s="4"/>
-      <c r="B135" s="4"/>
-      <c r="C135" s="4"/>
-      <c r="D135" s="4"/>
-      <c r="E135" s="4"/>
-      <c r="F135" s="4"/>
-      <c r="G135" s="4"/>
-      <c r="H135" s="4"/>
-      <c r="I135" s="4"/>
-      <c r="J135" s="4"/>
-      <c r="K135" s="4"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="13"/>
+      <c r="E135" s="13"/>
+      <c r="F135" s="13"/>
+      <c r="G135" s="13"/>
+      <c r="H135" s="13"/>
+      <c r="I135" s="13"/>
+      <c r="J135" s="13"/>
+      <c r="K135" s="13"/>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="s">
+      <c r="A136" s="13"/>
+      <c r="B136" s="13"/>
+      <c r="C136" s="13"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="13"/>
+      <c r="F136" s="13"/>
+      <c r="G136" s="13"/>
+      <c r="H136" s="13"/>
+      <c r="I136" s="13"/>
+      <c r="J136" s="13"/>
+      <c r="K136" s="13"/>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B136" s="3" t="s">
+      <c r="B137" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C136" s="3" t="s">
+      <c r="C137" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D136" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E136" s="3" t="s">
+      <c r="D137" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E137" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F136" s="3" t="s">
+      <c r="F137" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G136" s="3" t="s">
+      <c r="G137" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H136" s="3" t="s">
+      <c r="H137" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I136" s="3" t="s">
+      <c r="I137" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J136" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K136" s="3" t="s">
+      <c r="J137" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K137" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B137" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C137" s="7">
-        <v>4</v>
-      </c>
-      <c r="D137" s="7">
-        <v>10</v>
-      </c>
-      <c r="E137" s="7">
-        <v>0</v>
-      </c>
-      <c r="F137" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G137" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H137" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I137" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J137" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K137" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C138" s="7">
-        <v>200</v>
-      </c>
-      <c r="D138" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F138" s="11" t="s">
-        <v>20</v>
+        <v>4</v>
+      </c>
+      <c r="D138" s="7">
+        <v>10</v>
+      </c>
+      <c r="E138" s="7">
+        <v>0</v>
+      </c>
+      <c r="F138" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H138" s="7" t="s">
         <v>19</v>
@@ -3897,21 +3916,21 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C139" s="7">
-        <v>4</v>
-      </c>
-      <c r="D139" s="3">
-        <v>10</v>
-      </c>
-      <c r="E139" s="3">
-        <v>0</v>
-      </c>
-      <c r="F139" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F139" s="16" t="s">
         <v>19</v>
       </c>
       <c r="G139" s="7" t="s">
@@ -3931,34 +3950,34 @@
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A142" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B142" s="4" t="s">
+      <c r="A142" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B142" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C142" s="4"/>
-      <c r="D142" s="4"/>
-      <c r="E142" s="4"/>
-      <c r="F142" s="4"/>
-      <c r="G142" s="4"/>
-      <c r="H142" s="4"/>
-      <c r="I142" s="4"/>
-      <c r="J142" s="4"/>
-      <c r="K142" s="4"/>
+      <c r="C142" s="13"/>
+      <c r="D142" s="13"/>
+      <c r="E142" s="13"/>
+      <c r="F142" s="13"/>
+      <c r="G142" s="13"/>
+      <c r="H142" s="13"/>
+      <c r="I142" s="13"/>
+      <c r="J142" s="13"/>
+      <c r="K142" s="13"/>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A143" s="4"/>
-      <c r="B143" s="4"/>
-      <c r="C143" s="4"/>
-      <c r="D143" s="4"/>
-      <c r="E143" s="4"/>
-      <c r="F143" s="4"/>
-      <c r="G143" s="4"/>
-      <c r="H143" s="4"/>
-      <c r="I143" s="4"/>
-      <c r="J143" s="4"/>
-      <c r="K143" s="4"/>
+      <c r="A143" s="13"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="13"/>
+      <c r="F143" s="13"/>
+      <c r="G143" s="13"/>
+      <c r="H143" s="13"/>
+      <c r="I143" s="13"/>
+      <c r="J143" s="13"/>
+      <c r="K143" s="13"/>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
@@ -4014,7 +4033,7 @@
       <c r="F145" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G145" s="11" t="s">
+      <c r="G145" s="16" t="s">
         <v>20</v>
       </c>
       <c r="H145" s="7" t="s">
@@ -4049,7 +4068,7 @@
       <c r="F146" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G146" s="11" t="s">
+      <c r="G146" s="16" t="s">
         <v>20</v>
       </c>
       <c r="H146" s="7" t="s">
@@ -4116,7 +4135,7 @@
       <c r="E148" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F148" s="11" t="s">
+      <c r="F148" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G148" s="7" t="s">
@@ -4151,7 +4170,7 @@
       <c r="E149" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F149" s="11" t="s">
+      <c r="F149" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G149" s="7" t="s">
@@ -4172,44 +4191,44 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:K143"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="B116:K117"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="B126:K127"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="B134:K135"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="B91:K92"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="B99:K100"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="B106:K107"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:K63"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="B73:K74"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B82:K83"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:K3"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:K11"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:K21"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="B40:K41"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:K48"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B55:K56"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:K3"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:K11"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:K21"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:K64"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:K75"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:K84"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:K93"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="B100:K101"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="B107:K108"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="B142:K143"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="B117:K118"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="B127:K128"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B135:K136"/>
   </mergeCells>
-  <conditionalFormatting sqref="J78:K78">
-    <cfRule type="uniqueValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="J79:K79">
+    <cfRule type="uniqueValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J79:K79">
-    <cfRule type="uniqueValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="J80:K80">
+    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
alteracao valores dicionario de dados
</commit_message>
<xml_diff>
--- a/Banco de Dados/Dicionário_de_Dados.xlsx
+++ b/Banco de Dados/Dicionário_de_Dados.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gui\Documents\FloatGroup\FloatGroup\Banco de Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thaysa\Documents\4ºSemestre\InterDisiplinar\FloatGroup\FloatGroup\Banco de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7740"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="89">
   <si>
     <t>Tabela</t>
   </si>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>dataInicial</t>
+  </si>
+  <si>
+    <t>dataFinal</t>
   </si>
 </sst>
 </file>
@@ -394,9 +400,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -405,6 +408,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K149"/>
+  <dimension ref="A2:K151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,34 +728,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -892,34 +898,34 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1007,7 +1013,7 @@
       <c r="E14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="13" t="s">
         <v>19</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -1132,34 +1138,34 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1346,22 +1352,22 @@
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K27" s="8" t="s">
+      <c r="F27" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K27" s="13" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1716,34 +1722,34 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="13" t="s">
+      <c r="A40" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
@@ -1851,34 +1857,34 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="13" t="s">
+      <c r="A47" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
@@ -1966,7 +1972,7 @@
       <c r="E51" s="3">
         <v>2</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="F51" s="13" t="s">
         <v>19</v>
       </c>
       <c r="G51" s="3" t="s">
@@ -2001,7 +2007,7 @@
       <c r="E52" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="F52" s="13" t="s">
         <v>19</v>
       </c>
       <c r="G52" s="3" t="s">
@@ -2021,34 +2027,34 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="13" t="s">
+      <c r="A55" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="13"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="13"/>
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
@@ -2171,7 +2177,7 @@
       <c r="E60" s="4">
         <v>2</v>
       </c>
-      <c r="F60" s="14" t="s">
+      <c r="F60" s="13" t="s">
         <v>19</v>
       </c>
       <c r="G60" s="4" t="s">
@@ -2191,34 +2197,34 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="13" t="s">
+      <c r="A63" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="16"/>
+      <c r="K63" s="16"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13"/>
-      <c r="K64" s="13"/>
+      <c r="A64" s="16"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+      <c r="I64" s="16"/>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
@@ -2466,34 +2472,34 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B74" s="13" t="s">
+      <c r="A74" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="16"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="13"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="13"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
+      <c r="A75" s="16"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
+      <c r="J75" s="16"/>
+      <c r="K75" s="16"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
@@ -2667,34 +2673,34 @@
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B83" s="13" t="s">
+      <c r="A83" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13"/>
-      <c r="K83" s="13"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="16"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="16"/>
+      <c r="I83" s="16"/>
+      <c r="J83" s="16"/>
+      <c r="K83" s="16"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="13"/>
-      <c r="K84" s="13"/>
+      <c r="A84" s="16"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16"/>
+      <c r="I84" s="16"/>
+      <c r="J84" s="16"/>
+      <c r="K84" s="16"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
@@ -2866,34 +2872,34 @@
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B92" s="13" t="s">
+      <c r="A92" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C92" s="13"/>
-      <c r="D92" s="13"/>
-      <c r="E92" s="13"/>
-      <c r="F92" s="13"/>
-      <c r="G92" s="13"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13"/>
-      <c r="K92" s="13"/>
+      <c r="C92" s="16"/>
+      <c r="D92" s="16"/>
+      <c r="E92" s="16"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="16"/>
+      <c r="H92" s="16"/>
+      <c r="I92" s="16"/>
+      <c r="J92" s="16"/>
+      <c r="K92" s="16"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="13"/>
-      <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
-      <c r="D93" s="13"/>
-      <c r="E93" s="13"/>
-      <c r="F93" s="13"/>
-      <c r="G93" s="13"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="13"/>
-      <c r="K93" s="13"/>
+      <c r="A93" s="16"/>
+      <c r="B93" s="16"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="16"/>
+      <c r="E93" s="16"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="16"/>
+      <c r="H93" s="16"/>
+      <c r="I93" s="16"/>
+      <c r="J93" s="16"/>
+      <c r="K93" s="16"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
@@ -3001,313 +3007,301 @@
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G97" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H97" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I97" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J97" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K97" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G98" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H98" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I98" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J98" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K98" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B97" s="7" t="s">
+      <c r="B99" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C97" s="7">
+      <c r="C99" s="7">
         <v>5</v>
       </c>
-      <c r="D97" s="3">
+      <c r="D99" s="3">
         <v>15</v>
       </c>
-      <c r="E97" s="3">
+      <c r="E99" s="3">
         <v>2</v>
       </c>
-      <c r="F97" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G97" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H97" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I97" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J97" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K97" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B100" s="13" t="s">
+      <c r="F99" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H99" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I99" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J99" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K99" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C100" s="13"/>
-      <c r="D100" s="13"/>
-      <c r="E100" s="13"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
-      <c r="J100" s="13"/>
-      <c r="K100" s="13"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101" s="13"/>
-      <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
-      <c r="D101" s="13"/>
-      <c r="E101" s="13"/>
-      <c r="F101" s="13"/>
-      <c r="G101" s="13"/>
-      <c r="H101" s="13"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="13"/>
-      <c r="K101" s="13"/>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
+      <c r="C102" s="16"/>
+      <c r="D102" s="16"/>
+      <c r="E102" s="16"/>
+      <c r="F102" s="16"/>
+      <c r="G102" s="16"/>
+      <c r="H102" s="16"/>
+      <c r="I102" s="16"/>
+      <c r="J102" s="16"/>
+      <c r="K102" s="16"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="16"/>
+      <c r="B103" s="16"/>
+      <c r="C103" s="16"/>
+      <c r="D103" s="16"/>
+      <c r="E103" s="16"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="16"/>
+      <c r="H103" s="16"/>
+      <c r="I103" s="16"/>
+      <c r="J103" s="16"/>
+      <c r="K103" s="16"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B104" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D102" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E102" s="3" t="s">
+      <c r="D104" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E104" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F102" s="3" t="s">
+      <c r="F104" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G102" s="3" t="s">
+      <c r="G104" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H102" s="3" t="s">
+      <c r="H104" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I102" s="3" t="s">
+      <c r="I104" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J102" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K102" s="3" t="s">
+      <c r="J104" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K104" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B105" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C103" s="7">
-        <v>4</v>
-      </c>
-      <c r="D103" s="7">
-        <v>10</v>
-      </c>
-      <c r="E103" s="7">
-        <v>0</v>
-      </c>
-      <c r="F103" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G103" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H103" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I103" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J103" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K103" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
+      <c r="C105" s="7">
+        <v>4</v>
+      </c>
+      <c r="D105" s="7">
+        <v>10</v>
+      </c>
+      <c r="E105" s="7">
+        <v>0</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G105" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H105" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I105" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J105" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K105" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B106" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C104" s="3">
+      <c r="C106" s="3">
         <v>80</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F104" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G104" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H104" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I104" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J104" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K104" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B107" s="13" t="s">
+      <c r="D106" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F106" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G106" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K106" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C107" s="13"/>
-      <c r="D107" s="13"/>
-      <c r="E107" s="13"/>
-      <c r="F107" s="13"/>
-      <c r="G107" s="13"/>
-      <c r="H107" s="13"/>
-      <c r="I107" s="13"/>
-      <c r="J107" s="13"/>
-      <c r="K107" s="13"/>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A108" s="13"/>
-      <c r="B108" s="13"/>
-      <c r="C108" s="13"/>
-      <c r="D108" s="13"/>
-      <c r="E108" s="13"/>
-      <c r="F108" s="13"/>
-      <c r="G108" s="13"/>
-      <c r="H108" s="13"/>
-      <c r="I108" s="13"/>
-      <c r="J108" s="13"/>
-      <c r="K108" s="13"/>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
+      <c r="C109" s="16"/>
+      <c r="D109" s="16"/>
+      <c r="E109" s="16"/>
+      <c r="F109" s="16"/>
+      <c r="G109" s="16"/>
+      <c r="H109" s="16"/>
+      <c r="I109" s="16"/>
+      <c r="J109" s="16"/>
+      <c r="K109" s="16"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" s="16"/>
+      <c r="B110" s="16"/>
+      <c r="C110" s="16"/>
+      <c r="D110" s="16"/>
+      <c r="E110" s="16"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="16"/>
+      <c r="H110" s="16"/>
+      <c r="I110" s="16"/>
+      <c r="J110" s="16"/>
+      <c r="K110" s="16"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B111" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="C111" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E109" s="3" t="s">
+      <c r="D111" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E111" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F109" s="3" t="s">
+      <c r="F111" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G109" s="3" t="s">
+      <c r="G111" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H109" s="3" t="s">
+      <c r="H111" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I109" s="3" t="s">
+      <c r="I111" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J109" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K109" s="3" t="s">
+      <c r="J111" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K111" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C110" s="7">
-        <v>4</v>
-      </c>
-      <c r="D110" s="7">
-        <v>10</v>
-      </c>
-      <c r="E110" s="7">
-        <v>0</v>
-      </c>
-      <c r="F110" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G110" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H110" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I110" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J110" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K110" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C111" s="7">
-        <v>4</v>
-      </c>
-      <c r="D111" s="3">
-        <v>10</v>
-      </c>
-      <c r="E111" s="3">
-        <v>0</v>
-      </c>
-      <c r="F111" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G111" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H111" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I111" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J111" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="K111" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B112" s="7" t="s">
         <v>15</v>
@@ -3315,26 +3309,26 @@
       <c r="C112" s="7">
         <v>4</v>
       </c>
-      <c r="D112" s="3">
-        <v>10</v>
-      </c>
-      <c r="E112" s="3">
+      <c r="D112" s="7">
+        <v>10</v>
+      </c>
+      <c r="E112" s="7">
         <v>0</v>
       </c>
       <c r="F112" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G112" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I112" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J112" s="3" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="K112" s="3" t="s">
         <v>18</v>
@@ -3342,34 +3336,34 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C113" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D113" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E113" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F113" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G113" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H113" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I113" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J113" s="3" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="K113" s="3" t="s">
         <v>18</v>
@@ -3377,7 +3371,7 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="B114" s="7" t="s">
         <v>15</v>
@@ -3407,141 +3401,147 @@
         <v>18</v>
       </c>
       <c r="K114" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C115" s="7">
+        <v>5</v>
+      </c>
+      <c r="D115" s="3">
+        <v>15</v>
+      </c>
+      <c r="E115" s="3">
+        <v>2</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G115" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H115" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I115" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J115" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K115" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C116" s="7">
+        <v>4</v>
+      </c>
+      <c r="D116" s="3">
+        <v>10</v>
+      </c>
+      <c r="E116" s="3">
+        <v>0</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G116" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H116" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I116" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K116" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B117" s="13" t="s">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B119" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C117" s="13"/>
-      <c r="D117" s="13"/>
-      <c r="E117" s="13"/>
-      <c r="F117" s="13"/>
-      <c r="G117" s="13"/>
-      <c r="H117" s="13"/>
-      <c r="I117" s="13"/>
-      <c r="J117" s="13"/>
-      <c r="K117" s="13"/>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A118" s="13"/>
-      <c r="B118" s="13"/>
-      <c r="C118" s="13"/>
-      <c r="D118" s="13"/>
-      <c r="E118" s="13"/>
-      <c r="F118" s="13"/>
-      <c r="G118" s="13"/>
-      <c r="H118" s="13"/>
-      <c r="I118" s="13"/>
-      <c r="J118" s="13"/>
-      <c r="K118" s="13"/>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
+      <c r="C119" s="16"/>
+      <c r="D119" s="16"/>
+      <c r="E119" s="16"/>
+      <c r="F119" s="16"/>
+      <c r="G119" s="16"/>
+      <c r="H119" s="16"/>
+      <c r="I119" s="16"/>
+      <c r="J119" s="16"/>
+      <c r="K119" s="16"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" s="16"/>
+      <c r="B120" s="16"/>
+      <c r="C120" s="16"/>
+      <c r="D120" s="16"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="16"/>
+      <c r="G120" s="16"/>
+      <c r="H120" s="16"/>
+      <c r="I120" s="16"/>
+      <c r="J120" s="16"/>
+      <c r="K120" s="16"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B121" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C121" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D119" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E119" s="3" t="s">
+      <c r="D121" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E121" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F119" s="3" t="s">
+      <c r="F121" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G119" s="3" t="s">
+      <c r="G121" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H119" s="3" t="s">
+      <c r="H121" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I119" s="3" t="s">
+      <c r="I121" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J119" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K119" s="3" t="s">
+      <c r="J121" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K121" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B120" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C120" s="7">
-        <v>4</v>
-      </c>
-      <c r="D120" s="7">
-        <v>10</v>
-      </c>
-      <c r="E120" s="7">
-        <v>0</v>
-      </c>
-      <c r="F120" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G120" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H120" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I120" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J120" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K120" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B121" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C121" s="11"/>
-      <c r="D121" s="8"/>
-      <c r="E121" s="8"/>
-      <c r="F121" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G121" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H121" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I121" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J121" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K121" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>15</v>
@@ -3549,17 +3549,17 @@
       <c r="C122" s="7">
         <v>4</v>
       </c>
-      <c r="D122" s="3">
-        <v>10</v>
-      </c>
-      <c r="E122" s="3">
+      <c r="D122" s="7">
+        <v>10</v>
+      </c>
+      <c r="E122" s="7">
         <v>0</v>
       </c>
       <c r="F122" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G122" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H122" s="7" t="s">
         <v>19</v>
@@ -3571,25 +3571,19 @@
         <v>18</v>
       </c>
       <c r="K122" s="3" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B123" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C123" s="7">
-        <v>4</v>
-      </c>
-      <c r="D123" s="3">
-        <v>10</v>
-      </c>
-      <c r="E123" s="3">
-        <v>0</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B123" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C123" s="11"/>
+      <c r="D123" s="8"/>
+      <c r="E123" s="8"/>
       <c r="F123" s="7" t="s">
         <v>19</v>
       </c>
@@ -3597,13 +3591,13 @@
         <v>19</v>
       </c>
       <c r="H123" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I123" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J123" s="3" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="K123" s="3" t="s">
         <v>18</v>
@@ -3611,7 +3605,7 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="B124" s="7" t="s">
         <v>15</v>
@@ -3619,10 +3613,10 @@
       <c r="C124" s="7">
         <v>4</v>
       </c>
-      <c r="D124" s="7">
-        <v>10</v>
-      </c>
-      <c r="E124" s="7">
+      <c r="D124" s="3">
+        <v>10</v>
+      </c>
+      <c r="E124" s="3">
         <v>0</v>
       </c>
       <c r="F124" s="7" t="s">
@@ -3632,156 +3626,156 @@
         <v>19</v>
       </c>
       <c r="H124" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I124" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J124" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K124" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C125" s="7">
+        <v>4</v>
+      </c>
+      <c r="D125" s="3">
+        <v>10</v>
+      </c>
+      <c r="E125" s="3">
+        <v>0</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G125" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I125" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J125" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K125" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C126" s="7">
+        <v>4</v>
+      </c>
+      <c r="D126" s="7">
+        <v>10</v>
+      </c>
+      <c r="E126" s="7">
+        <v>0</v>
+      </c>
+      <c r="F126" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G126" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H126" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I126" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J126" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K124" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A127" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B127" s="13" t="s">
+      <c r="K126" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A129" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B129" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C127" s="13"/>
-      <c r="D127" s="13"/>
-      <c r="E127" s="13"/>
-      <c r="F127" s="13"/>
-      <c r="G127" s="13"/>
-      <c r="H127" s="13"/>
-      <c r="I127" s="13"/>
-      <c r="J127" s="13"/>
-      <c r="K127" s="13"/>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A128" s="13"/>
-      <c r="B128" s="13"/>
-      <c r="C128" s="13"/>
-      <c r="D128" s="13"/>
-      <c r="E128" s="13"/>
-      <c r="F128" s="13"/>
-      <c r="G128" s="13"/>
-      <c r="H128" s="13"/>
-      <c r="I128" s="13"/>
-      <c r="J128" s="13"/>
-      <c r="K128" s="13"/>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
+      <c r="C129" s="16"/>
+      <c r="D129" s="16"/>
+      <c r="E129" s="16"/>
+      <c r="F129" s="16"/>
+      <c r="G129" s="16"/>
+      <c r="H129" s="16"/>
+      <c r="I129" s="16"/>
+      <c r="J129" s="16"/>
+      <c r="K129" s="16"/>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A130" s="16"/>
+      <c r="B130" s="16"/>
+      <c r="C130" s="16"/>
+      <c r="D130" s="16"/>
+      <c r="E130" s="16"/>
+      <c r="F130" s="16"/>
+      <c r="G130" s="16"/>
+      <c r="H130" s="16"/>
+      <c r="I130" s="16"/>
+      <c r="J130" s="16"/>
+      <c r="K130" s="16"/>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B129" s="3" t="s">
+      <c r="B131" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C129" s="3" t="s">
+      <c r="C131" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D129" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E129" s="3" t="s">
+      <c r="D131" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E131" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F129" s="3" t="s">
+      <c r="F131" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G129" s="3" t="s">
+      <c r="G131" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H129" s="3" t="s">
+      <c r="H131" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I129" s="3" t="s">
+      <c r="I131" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J129" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K129" s="3" t="s">
+      <c r="J131" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K131" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C130" s="7">
-        <v>4</v>
-      </c>
-      <c r="D130" s="7">
-        <v>10</v>
-      </c>
-      <c r="E130" s="7">
-        <v>0</v>
-      </c>
-      <c r="F130" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G130" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H130" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I130" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J130" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="K130" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B131" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C131" s="7">
-        <v>4</v>
-      </c>
-      <c r="D131" s="3">
-        <v>10</v>
-      </c>
-      <c r="E131" s="3">
-        <v>0</v>
-      </c>
-      <c r="F131" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G131" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H131" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I131" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J131" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="K131" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B132" s="7" t="s">
         <v>15</v>
@@ -3789,331 +3783,331 @@
       <c r="C132" s="7">
         <v>4</v>
       </c>
-      <c r="D132" s="3">
-        <v>10</v>
-      </c>
-      <c r="E132" s="3">
+      <c r="D132" s="7">
+        <v>10</v>
+      </c>
+      <c r="E132" s="7">
         <v>0</v>
       </c>
       <c r="F132" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G132" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I132" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J132" s="3" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="K132" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B135" s="13" t="s">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C133" s="7">
+        <v>4</v>
+      </c>
+      <c r="D133" s="3">
+        <v>10</v>
+      </c>
+      <c r="E133" s="3">
+        <v>0</v>
+      </c>
+      <c r="F133" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G133" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H133" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I133" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J133" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K133" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C134" s="7">
+        <v>4</v>
+      </c>
+      <c r="D134" s="3">
+        <v>10</v>
+      </c>
+      <c r="E134" s="3">
+        <v>0</v>
+      </c>
+      <c r="F134" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G134" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H134" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I134" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J134" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K134" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A137" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C135" s="13"/>
-      <c r="D135" s="13"/>
-      <c r="E135" s="13"/>
-      <c r="F135" s="13"/>
-      <c r="G135" s="13"/>
-      <c r="H135" s="13"/>
-      <c r="I135" s="13"/>
-      <c r="J135" s="13"/>
-      <c r="K135" s="13"/>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A136" s="13"/>
-      <c r="B136" s="13"/>
-      <c r="C136" s="13"/>
-      <c r="D136" s="13"/>
-      <c r="E136" s="13"/>
-      <c r="F136" s="13"/>
-      <c r="G136" s="13"/>
-      <c r="H136" s="13"/>
-      <c r="I136" s="13"/>
-      <c r="J136" s="13"/>
-      <c r="K136" s="13"/>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
+      <c r="C137" s="16"/>
+      <c r="D137" s="16"/>
+      <c r="E137" s="16"/>
+      <c r="F137" s="16"/>
+      <c r="G137" s="16"/>
+      <c r="H137" s="16"/>
+      <c r="I137" s="16"/>
+      <c r="J137" s="16"/>
+      <c r="K137" s="16"/>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A138" s="16"/>
+      <c r="B138" s="16"/>
+      <c r="C138" s="16"/>
+      <c r="D138" s="16"/>
+      <c r="E138" s="16"/>
+      <c r="F138" s="16"/>
+      <c r="G138" s="16"/>
+      <c r="H138" s="16"/>
+      <c r="I138" s="16"/>
+      <c r="J138" s="16"/>
+      <c r="K138" s="16"/>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B137" s="3" t="s">
+      <c r="B139" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C137" s="3" t="s">
+      <c r="C139" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D137" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E137" s="3" t="s">
+      <c r="D139" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E139" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F137" s="3" t="s">
+      <c r="F139" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G137" s="3" t="s">
+      <c r="G139" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H137" s="3" t="s">
+      <c r="H139" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I137" s="3" t="s">
+      <c r="I139" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J137" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K137" s="3" t="s">
+      <c r="J139" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K139" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B138" s="7" t="s">
+      <c r="B140" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C138" s="7">
-        <v>4</v>
-      </c>
-      <c r="D138" s="7">
-        <v>10</v>
-      </c>
-      <c r="E138" s="7">
-        <v>0</v>
-      </c>
-      <c r="F138" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G138" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H138" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I138" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J138" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K138" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
+      <c r="C140" s="7">
+        <v>4</v>
+      </c>
+      <c r="D140" s="7">
+        <v>10</v>
+      </c>
+      <c r="E140" s="7">
+        <v>0</v>
+      </c>
+      <c r="F140" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G140" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H140" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I140" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J140" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K140" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B139" s="7" t="s">
+      <c r="B141" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C139" s="7">
+      <c r="C141" s="7">
         <v>200</v>
       </c>
-      <c r="D139" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E139" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F139" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G139" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H139" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I139" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J139" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K139" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A142" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B142" s="13" t="s">
+      <c r="D141" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F141" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G141" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H141" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I141" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J141" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K141" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A144" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B144" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C142" s="13"/>
-      <c r="D142" s="13"/>
-      <c r="E142" s="13"/>
-      <c r="F142" s="13"/>
-      <c r="G142" s="13"/>
-      <c r="H142" s="13"/>
-      <c r="I142" s="13"/>
-      <c r="J142" s="13"/>
-      <c r="K142" s="13"/>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A143" s="13"/>
-      <c r="B143" s="13"/>
-      <c r="C143" s="13"/>
-      <c r="D143" s="13"/>
-      <c r="E143" s="13"/>
-      <c r="F143" s="13"/>
-      <c r="G143" s="13"/>
-      <c r="H143" s="13"/>
-      <c r="I143" s="13"/>
-      <c r="J143" s="13"/>
-      <c r="K143" s="13"/>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A144" s="3" t="s">
+      <c r="C144" s="16"/>
+      <c r="D144" s="16"/>
+      <c r="E144" s="16"/>
+      <c r="F144" s="16"/>
+      <c r="G144" s="16"/>
+      <c r="H144" s="16"/>
+      <c r="I144" s="16"/>
+      <c r="J144" s="16"/>
+      <c r="K144" s="16"/>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A145" s="16"/>
+      <c r="B145" s="16"/>
+      <c r="C145" s="16"/>
+      <c r="D145" s="16"/>
+      <c r="E145" s="16"/>
+      <c r="F145" s="16"/>
+      <c r="G145" s="16"/>
+      <c r="H145" s="16"/>
+      <c r="I145" s="16"/>
+      <c r="J145" s="16"/>
+      <c r="K145" s="16"/>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B146" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C144" s="3" t="s">
+      <c r="C146" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D144" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E144" s="3" t="s">
+      <c r="D146" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E146" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F144" s="3" t="s">
+      <c r="F146" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G144" s="3" t="s">
+      <c r="G146" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H144" s="3" t="s">
+      <c r="H146" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I144" s="3" t="s">
+      <c r="I146" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J144" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K144" s="3" t="s">
+      <c r="J146" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K146" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B145" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C145" s="7">
-        <v>4</v>
-      </c>
-      <c r="D145" s="7">
-        <v>10</v>
-      </c>
-      <c r="E145" s="7">
-        <v>0</v>
-      </c>
-      <c r="F145" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G145" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H145" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I145" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J145" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K145" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B146" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C146" s="7">
-        <v>4</v>
-      </c>
-      <c r="D146" s="3">
-        <v>10</v>
-      </c>
-      <c r="E146" s="3">
-        <v>0</v>
-      </c>
-      <c r="F146" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G146" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H146" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I146" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J146" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K146" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C147" s="7">
-        <v>10</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E147" s="3" t="s">
-        <v>18</v>
+        <v>4</v>
+      </c>
+      <c r="D147" s="7">
+        <v>10</v>
+      </c>
+      <c r="E147" s="7">
+        <v>0</v>
       </c>
       <c r="F147" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G147" s="7" t="s">
-        <v>19</v>
+      <c r="G147" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="H147" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I147" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J147" s="3" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="K147" s="3" t="s">
         <v>18</v>
@@ -4121,34 +4115,34 @@
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C148" s="7">
-        <v>100</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E148" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F148" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G148" s="7" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="D148" s="3">
+        <v>10</v>
+      </c>
+      <c r="E148" s="3">
+        <v>0</v>
+      </c>
+      <c r="F148" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G148" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="H148" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I148" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J148" s="3" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="K148" s="3" t="s">
         <v>18</v>
@@ -4156,73 +4150,143 @@
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B149" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C149" s="7">
+        <v>10</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F149" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G149" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H149" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I149" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J149" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K149" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C150" s="7">
         <v>100</v>
       </c>
-      <c r="D149" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F149" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G149" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H149" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I149" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J149" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K149" s="3" t="s">
+      <c r="D150" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F150" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G150" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H150" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I150" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J150" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K150" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C151" s="7">
+        <v>100</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F151" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G151" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H151" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I151" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J151" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K151" s="3" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A144:A145"/>
+    <mergeCell ref="B144:K145"/>
+    <mergeCell ref="A119:A120"/>
+    <mergeCell ref="B119:K120"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="B129:K130"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="B137:K138"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:K93"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="B102:K103"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="B109:K110"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:K64"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:K75"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:K84"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:K41"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:K48"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:K56"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:K3"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:K11"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:K21"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:K41"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:K48"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:K56"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:K64"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:K75"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:K84"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:K93"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="B100:K101"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="B107:K108"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:K143"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="B117:K118"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="B127:K128"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B135:K136"/>
   </mergeCells>
   <conditionalFormatting sqref="J79:K79">
     <cfRule type="uniqueValues" dxfId="1" priority="2"/>

</xml_diff>

<commit_message>
remoção dos medicamentos do sistema, correção da view v_agenda e alguns ajustes na DDL, diagramas e dicionário de dados
</commit_message>
<xml_diff>
--- a/Banco de Dados/Dicionário_de_Dados.xlsx
+++ b/Banco de Dados/Dicionário_de_Dados.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thaysa\Documents\4ºSemestre\InterDisiplinar\FloatGroup\FloatGroup\Banco de Dados\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="88">
   <si>
     <t>Tabela</t>
   </si>
@@ -279,9 +274,6 @@
   </si>
   <si>
     <t>periodo</t>
-  </si>
-  <si>
-    <t>blob</t>
   </si>
   <si>
     <t>max</t>
@@ -366,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -408,6 +400,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -705,7 +700,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -713,49 +708,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K151"/>
+  <dimension ref="A2:K152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27:K27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="9.140625" style="1"/>
+    <col min="2" max="2" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -898,34 +894,34 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="16" t="s">
+      <c r="A10" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1138,34 +1134,34 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="16" t="s">
+      <c r="A20" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1353,7 +1349,7 @@
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>19</v>
@@ -1722,34 +1718,34 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="16" t="s">
+      <c r="A40" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="16"/>
-      <c r="K40" s="16"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
@@ -1857,34 +1853,34 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="16" t="s">
+      <c r="A47" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="16"/>
-      <c r="K47" s="16"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="I48" s="16"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="16"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
@@ -2027,34 +2023,34 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="16" t="s">
+      <c r="A55" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="16"/>
-      <c r="I55" s="16"/>
-      <c r="J55" s="16"/>
-      <c r="K55" s="16"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="16"/>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
@@ -2197,34 +2193,34 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="16" t="s">
+      <c r="A63" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="16"/>
-      <c r="K63" s="16"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
-      <c r="I64" s="16"/>
-      <c r="J64" s="16"/>
-      <c r="K64" s="16"/>
+      <c r="A64" s="17"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
+      <c r="K64" s="17"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
@@ -2472,34 +2468,34 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B74" s="16" t="s">
+      <c r="A74" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C74" s="16"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="16"/>
-      <c r="I74" s="16"/>
-      <c r="J74" s="16"/>
-      <c r="K74" s="16"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
+      <c r="J74" s="17"/>
+      <c r="K74" s="17"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="16"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="16"/>
-      <c r="D75" s="16"/>
-      <c r="E75" s="16"/>
-      <c r="F75" s="16"/>
-      <c r="G75" s="16"/>
-      <c r="H75" s="16"/>
-      <c r="I75" s="16"/>
-      <c r="J75" s="16"/>
-      <c r="K75" s="16"/>
+      <c r="A75" s="17"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
+      <c r="J75" s="17"/>
+      <c r="K75" s="17"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
@@ -2646,13 +2642,17 @@
         <v>59</v>
       </c>
       <c r="B80" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C80" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C80" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
+      <c r="D80" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E80" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="F80" s="11" t="s">
         <v>19</v>
       </c>
@@ -2673,34 +2673,34 @@
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B83" s="16" t="s">
+      <c r="A83" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C83" s="16"/>
-      <c r="D83" s="16"/>
-      <c r="E83" s="16"/>
-      <c r="F83" s="16"/>
-      <c r="G83" s="16"/>
-      <c r="H83" s="16"/>
-      <c r="I83" s="16"/>
-      <c r="J83" s="16"/>
-      <c r="K83" s="16"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="17"/>
+      <c r="H83" s="17"/>
+      <c r="I83" s="17"/>
+      <c r="J83" s="17"/>
+      <c r="K83" s="17"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="16"/>
-      <c r="B84" s="16"/>
-      <c r="C84" s="16"/>
-      <c r="D84" s="16"/>
-      <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
-      <c r="G84" s="16"/>
-      <c r="H84" s="16"/>
-      <c r="I84" s="16"/>
-      <c r="J84" s="16"/>
-      <c r="K84" s="16"/>
+      <c r="A84" s="17"/>
+      <c r="B84" s="17"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="17"/>
+      <c r="I84" s="17"/>
+      <c r="J84" s="17"/>
+      <c r="K84" s="17"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
@@ -2846,10 +2846,10 @@
       <c r="C89" s="7">
         <v>4</v>
       </c>
-      <c r="D89" s="3">
-        <v>10</v>
-      </c>
-      <c r="E89" s="3">
+      <c r="D89" s="16">
+        <v>10</v>
+      </c>
+      <c r="E89" s="16">
         <v>0</v>
       </c>
       <c r="F89" s="12" t="s">
@@ -2867,177 +2867,183 @@
       <c r="J89" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K89" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B92" s="16" t="s">
+      <c r="K89" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" s="7">
+        <v>4</v>
+      </c>
+      <c r="D90" s="3">
+        <v>10</v>
+      </c>
+      <c r="E90" s="3">
+        <v>0</v>
+      </c>
+      <c r="F90" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G90" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H90" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I90" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J90" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K90" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C92" s="16"/>
-      <c r="D92" s="16"/>
-      <c r="E92" s="16"/>
-      <c r="F92" s="16"/>
-      <c r="G92" s="16"/>
-      <c r="H92" s="16"/>
-      <c r="I92" s="16"/>
-      <c r="J92" s="16"/>
-      <c r="K92" s="16"/>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="16"/>
-      <c r="B93" s="16"/>
-      <c r="C93" s="16"/>
-      <c r="D93" s="16"/>
-      <c r="E93" s="16"/>
-      <c r="F93" s="16"/>
-      <c r="G93" s="16"/>
-      <c r="H93" s="16"/>
-      <c r="I93" s="16"/>
-      <c r="J93" s="16"/>
-      <c r="K93" s="16"/>
+      <c r="C93" s="17"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="17"/>
+      <c r="F93" s="17"/>
+      <c r="G93" s="17"/>
+      <c r="H93" s="17"/>
+      <c r="I93" s="17"/>
+      <c r="J93" s="17"/>
+      <c r="K93" s="17"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="17"/>
+      <c r="B94" s="17"/>
+      <c r="C94" s="17"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="17"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="17"/>
+      <c r="H94" s="17"/>
+      <c r="I94" s="17"/>
+      <c r="J94" s="17"/>
+      <c r="K94" s="17"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B95" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E94" s="3" t="s">
+      <c r="D95" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E95" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F94" s="3" t="s">
+      <c r="F95" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G94" s="3" t="s">
+      <c r="G95" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H94" s="3" t="s">
+      <c r="H95" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I94" s="3" t="s">
+      <c r="I95" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J94" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K94" s="3" t="s">
+      <c r="J95" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K95" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B95" s="7" t="s">
+      <c r="B96" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C95" s="7">
-        <v>4</v>
-      </c>
-      <c r="D95" s="7">
-        <v>10</v>
-      </c>
-      <c r="E95" s="7">
-        <v>0</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G95" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H95" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I95" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J95" s="3" t="s">
+      <c r="C96" s="7">
+        <v>4</v>
+      </c>
+      <c r="D96" s="7">
+        <v>10</v>
+      </c>
+      <c r="E96" s="7">
+        <v>0</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G96" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H96" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I96" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J96" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K95" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C96" s="3">
-        <v>4</v>
-      </c>
-      <c r="D96" s="3">
-        <v>10</v>
-      </c>
-      <c r="E96" s="3">
-        <v>0</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G96" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I96" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J96" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="K96" s="3" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C97" s="8"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G97" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H97" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I97" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J97" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="K97" s="13" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" s="3">
+        <v>4</v>
+      </c>
+      <c r="D97" s="3">
+        <v>10</v>
+      </c>
+      <c r="E97" s="3">
+        <v>0</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J97" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K97" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>88</v>
+      <c r="A98" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>40</v>
@@ -3066,277 +3072,271 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G99" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H99" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I99" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J99" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K99" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B99" s="7" t="s">
+      <c r="B100" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C99" s="7">
+      <c r="C100" s="7">
         <v>5</v>
       </c>
-      <c r="D99" s="3">
+      <c r="D100" s="3">
         <v>15</v>
       </c>
-      <c r="E99" s="3">
+      <c r="E100" s="3">
         <v>2</v>
       </c>
-      <c r="F99" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G99" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H99" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I99" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J99" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K99" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B102" s="16" t="s">
+      <c r="F100" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G100" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H100" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I100" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J100" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C102" s="16"/>
-      <c r="D102" s="16"/>
-      <c r="E102" s="16"/>
-      <c r="F102" s="16"/>
-      <c r="G102" s="16"/>
-      <c r="H102" s="16"/>
-      <c r="I102" s="16"/>
-      <c r="J102" s="16"/>
-      <c r="K102" s="16"/>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="16"/>
-      <c r="B103" s="16"/>
-      <c r="C103" s="16"/>
-      <c r="D103" s="16"/>
-      <c r="E103" s="16"/>
-      <c r="F103" s="16"/>
-      <c r="G103" s="16"/>
-      <c r="H103" s="16"/>
-      <c r="I103" s="16"/>
-      <c r="J103" s="16"/>
-      <c r="K103" s="16"/>
+      <c r="C103" s="17"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="17"/>
+      <c r="F103" s="17"/>
+      <c r="G103" s="17"/>
+      <c r="H103" s="17"/>
+      <c r="I103" s="17"/>
+      <c r="J103" s="17"/>
+      <c r="K103" s="17"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
+      <c r="A104" s="17"/>
+      <c r="B104" s="17"/>
+      <c r="C104" s="17"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="17"/>
+      <c r="F104" s="17"/>
+      <c r="G104" s="17"/>
+      <c r="H104" s="17"/>
+      <c r="I104" s="17"/>
+      <c r="J104" s="17"/>
+      <c r="K104" s="17"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E104" s="3" t="s">
+      <c r="D105" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E105" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F104" s="3" t="s">
+      <c r="F105" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G104" s="3" t="s">
+      <c r="G105" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H104" s="3" t="s">
+      <c r="H105" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I104" s="3" t="s">
+      <c r="I105" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J104" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K104" s="3" t="s">
+      <c r="J105" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K105" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B105" s="7" t="s">
+      <c r="B106" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C105" s="7">
-        <v>4</v>
-      </c>
-      <c r="D105" s="7">
-        <v>10</v>
-      </c>
-      <c r="E105" s="7">
-        <v>0</v>
-      </c>
-      <c r="F105" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G105" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H105" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I105" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J105" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K105" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+      <c r="C106" s="7">
+        <v>4</v>
+      </c>
+      <c r="D106" s="7">
+        <v>10</v>
+      </c>
+      <c r="E106" s="7">
+        <v>0</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G106" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H106" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I106" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K106" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C106" s="3">
+      <c r="C107" s="3">
         <v>80</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F106" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G106" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H106" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I106" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J106" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K106" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B109" s="16" t="s">
+      <c r="D107" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F107" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G107" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H107" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I107" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J107" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K107" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C109" s="16"/>
-      <c r="D109" s="16"/>
-      <c r="E109" s="16"/>
-      <c r="F109" s="16"/>
-      <c r="G109" s="16"/>
-      <c r="H109" s="16"/>
-      <c r="I109" s="16"/>
-      <c r="J109" s="16"/>
-      <c r="K109" s="16"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A110" s="16"/>
-      <c r="B110" s="16"/>
-      <c r="C110" s="16"/>
-      <c r="D110" s="16"/>
-      <c r="E110" s="16"/>
-      <c r="F110" s="16"/>
-      <c r="G110" s="16"/>
-      <c r="H110" s="16"/>
-      <c r="I110" s="16"/>
-      <c r="J110" s="16"/>
-      <c r="K110" s="16"/>
+      <c r="C110" s="17"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="17"/>
+      <c r="F110" s="17"/>
+      <c r="G110" s="17"/>
+      <c r="H110" s="17"/>
+      <c r="I110" s="17"/>
+      <c r="J110" s="17"/>
+      <c r="K110" s="17"/>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="17"/>
+      <c r="B111" s="17"/>
+      <c r="C111" s="17"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="17"/>
+      <c r="F111" s="17"/>
+      <c r="G111" s="17"/>
+      <c r="H111" s="17"/>
+      <c r="I111" s="17"/>
+      <c r="J111" s="17"/>
+      <c r="K111" s="17"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B112" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C112" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D111" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E111" s="3" t="s">
+      <c r="D112" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E112" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F111" s="3" t="s">
+      <c r="F112" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G111" s="3" t="s">
+      <c r="G112" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H111" s="3" t="s">
+      <c r="H112" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I111" s="3" t="s">
+      <c r="I112" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J111" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K111" s="3" t="s">
+      <c r="J112" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K112" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B112" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C112" s="7">
-        <v>4</v>
-      </c>
-      <c r="D112" s="7">
-        <v>10</v>
-      </c>
-      <c r="E112" s="7">
-        <v>0</v>
-      </c>
-      <c r="F112" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G112" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H112" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I112" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J112" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K112" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B113" s="7" t="s">
         <v>15</v>
@@ -3344,10 +3344,10 @@
       <c r="C113" s="7">
         <v>4</v>
       </c>
-      <c r="D113" s="3">
-        <v>10</v>
-      </c>
-      <c r="E113" s="3">
+      <c r="D113" s="7">
+        <v>10</v>
+      </c>
+      <c r="E113" s="7">
         <v>0</v>
       </c>
       <c r="F113" s="7" t="s">
@@ -3363,7 +3363,7 @@
         <v>19</v>
       </c>
       <c r="J113" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K113" s="3" t="s">
         <v>18</v>
@@ -3371,7 +3371,7 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B114" s="7" t="s">
         <v>15</v>
@@ -3389,16 +3389,16 @@
         <v>19</v>
       </c>
       <c r="G114" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I114" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J114" s="3" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="K114" s="3" t="s">
         <v>18</v>
@@ -3406,22 +3406,22 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C115" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D115" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E115" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G115" s="7" t="s">
         <v>19</v>
@@ -3441,154 +3441,160 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C116" s="7">
+        <v>5</v>
+      </c>
+      <c r="D116" s="3">
+        <v>15</v>
+      </c>
+      <c r="E116" s="3">
+        <v>2</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G116" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H116" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I116" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K116" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B116" s="7" t="s">
+      <c r="B117" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C116" s="7">
-        <v>4</v>
-      </c>
-      <c r="D116" s="3">
-        <v>10</v>
-      </c>
-      <c r="E116" s="3">
-        <v>0</v>
-      </c>
-      <c r="F116" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G116" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H116" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I116" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J116" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K116" s="3" t="s">
+      <c r="C117" s="7">
+        <v>4</v>
+      </c>
+      <c r="D117" s="3">
+        <v>10</v>
+      </c>
+      <c r="E117" s="3">
+        <v>0</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G117" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H117" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I117" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J117" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K117" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B119" s="16" t="s">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B120" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C119" s="16"/>
-      <c r="D119" s="16"/>
-      <c r="E119" s="16"/>
-      <c r="F119" s="16"/>
-      <c r="G119" s="16"/>
-      <c r="H119" s="16"/>
-      <c r="I119" s="16"/>
-      <c r="J119" s="16"/>
-      <c r="K119" s="16"/>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A120" s="16"/>
-      <c r="B120" s="16"/>
-      <c r="C120" s="16"/>
-      <c r="D120" s="16"/>
-      <c r="E120" s="16"/>
-      <c r="F120" s="16"/>
-      <c r="G120" s="16"/>
-      <c r="H120" s="16"/>
-      <c r="I120" s="16"/>
-      <c r="J120" s="16"/>
-      <c r="K120" s="16"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="17"/>
+      <c r="G120" s="17"/>
+      <c r="H120" s="17"/>
+      <c r="I120" s="17"/>
+      <c r="J120" s="17"/>
+      <c r="K120" s="17"/>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
+      <c r="A121" s="17"/>
+      <c r="B121" s="17"/>
+      <c r="C121" s="17"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="17"/>
+      <c r="F121" s="17"/>
+      <c r="G121" s="17"/>
+      <c r="H121" s="17"/>
+      <c r="I121" s="17"/>
+      <c r="J121" s="17"/>
+      <c r="K121" s="17"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B122" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="C122" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D121" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E121" s="3" t="s">
+      <c r="D122" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E122" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F121" s="3" t="s">
+      <c r="F122" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G121" s="3" t="s">
+      <c r="G122" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H121" s="3" t="s">
+      <c r="H122" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I121" s="3" t="s">
+      <c r="I122" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J121" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K121" s="3" t="s">
+      <c r="J122" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K122" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B122" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C122" s="7">
-        <v>4</v>
-      </c>
-      <c r="D122" s="7">
-        <v>10</v>
-      </c>
-      <c r="E122" s="7">
-        <v>0</v>
-      </c>
-      <c r="F122" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G122" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H122" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I122" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J122" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K122" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B123" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C123" s="11"/>
-      <c r="D123" s="8"/>
-      <c r="E123" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C123" s="7">
+        <v>4</v>
+      </c>
+      <c r="D123" s="7">
+        <v>10</v>
+      </c>
+      <c r="E123" s="7">
+        <v>0</v>
+      </c>
       <c r="F123" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G123" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H123" s="7" t="s">
         <v>19</v>
@@ -3605,20 +3611,14 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B124" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C124" s="7">
-        <v>4</v>
-      </c>
-      <c r="D124" s="3">
-        <v>10</v>
-      </c>
-      <c r="E124" s="3">
-        <v>0</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B124" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C124" s="11"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8"/>
       <c r="F124" s="7" t="s">
         <v>19</v>
       </c>
@@ -3635,12 +3635,12 @@
         <v>18</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B125" s="7" t="s">
         <v>15</v>
@@ -3661,21 +3661,21 @@
         <v>19</v>
       </c>
       <c r="H125" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I125" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J125" s="3" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="K125" s="3" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B126" s="7" t="s">
         <v>15</v>
@@ -3683,10 +3683,10 @@
       <c r="C126" s="7">
         <v>4</v>
       </c>
-      <c r="D126" s="7">
-        <v>10</v>
-      </c>
-      <c r="E126" s="7">
+      <c r="D126" s="3">
+        <v>10</v>
+      </c>
+      <c r="E126" s="3">
         <v>0</v>
       </c>
       <c r="F126" s="7" t="s">
@@ -3702,115 +3702,115 @@
         <v>19</v>
       </c>
       <c r="J126" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K126" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C127" s="7">
+        <v>4</v>
+      </c>
+      <c r="D127" s="7">
+        <v>10</v>
+      </c>
+      <c r="E127" s="7">
+        <v>0</v>
+      </c>
+      <c r="F127" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G127" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I127" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J127" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K126" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B129" s="16" t="s">
+      <c r="K127" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A130" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B130" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C129" s="16"/>
-      <c r="D129" s="16"/>
-      <c r="E129" s="16"/>
-      <c r="F129" s="16"/>
-      <c r="G129" s="16"/>
-      <c r="H129" s="16"/>
-      <c r="I129" s="16"/>
-      <c r="J129" s="16"/>
-      <c r="K129" s="16"/>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A130" s="16"/>
-      <c r="B130" s="16"/>
-      <c r="C130" s="16"/>
-      <c r="D130" s="16"/>
-      <c r="E130" s="16"/>
-      <c r="F130" s="16"/>
-      <c r="G130" s="16"/>
-      <c r="H130" s="16"/>
-      <c r="I130" s="16"/>
-      <c r="J130" s="16"/>
-      <c r="K130" s="16"/>
+      <c r="C130" s="17"/>
+      <c r="D130" s="17"/>
+      <c r="E130" s="17"/>
+      <c r="F130" s="17"/>
+      <c r="G130" s="17"/>
+      <c r="H130" s="17"/>
+      <c r="I130" s="17"/>
+      <c r="J130" s="17"/>
+      <c r="K130" s="17"/>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
+      <c r="A131" s="17"/>
+      <c r="B131" s="17"/>
+      <c r="C131" s="17"/>
+      <c r="D131" s="17"/>
+      <c r="E131" s="17"/>
+      <c r="F131" s="17"/>
+      <c r="G131" s="17"/>
+      <c r="H131" s="17"/>
+      <c r="I131" s="17"/>
+      <c r="J131" s="17"/>
+      <c r="K131" s="17"/>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B131" s="3" t="s">
+      <c r="B132" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C131" s="3" t="s">
+      <c r="C132" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D131" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E131" s="3" t="s">
+      <c r="D132" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E132" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F131" s="3" t="s">
+      <c r="F132" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G131" s="3" t="s">
+      <c r="G132" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H131" s="3" t="s">
+      <c r="H132" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I131" s="3" t="s">
+      <c r="I132" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J131" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K131" s="3" t="s">
+      <c r="J132" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K132" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B132" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C132" s="7">
-        <v>4</v>
-      </c>
-      <c r="D132" s="7">
-        <v>10</v>
-      </c>
-      <c r="E132" s="7">
-        <v>0</v>
-      </c>
-      <c r="F132" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G132" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H132" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I132" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J132" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="K132" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B133" s="7" t="s">
         <v>15</v>
@@ -3818,10 +3818,10 @@
       <c r="C133" s="7">
         <v>4</v>
       </c>
-      <c r="D133" s="3">
-        <v>10</v>
-      </c>
-      <c r="E133" s="3">
+      <c r="D133" s="7">
+        <v>10</v>
+      </c>
+      <c r="E133" s="7">
         <v>0</v>
       </c>
       <c r="F133" s="7" t="s">
@@ -3837,7 +3837,7 @@
         <v>19</v>
       </c>
       <c r="J133" s="3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="K133" s="3" t="s">
         <v>18</v>
@@ -3845,7 +3845,7 @@
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B134" s="7" t="s">
         <v>15</v>
@@ -3863,259 +3863,259 @@
         <v>19</v>
       </c>
       <c r="G134" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H134" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I134" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J134" s="3" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="K134" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A137" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B137" s="16" t="s">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C135" s="7">
+        <v>4</v>
+      </c>
+      <c r="D135" s="3">
+        <v>10</v>
+      </c>
+      <c r="E135" s="3">
+        <v>0</v>
+      </c>
+      <c r="F135" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G135" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H135" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I135" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J135" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K135" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A138" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B138" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C137" s="16"/>
-      <c r="D137" s="16"/>
-      <c r="E137" s="16"/>
-      <c r="F137" s="16"/>
-      <c r="G137" s="16"/>
-      <c r="H137" s="16"/>
-      <c r="I137" s="16"/>
-      <c r="J137" s="16"/>
-      <c r="K137" s="16"/>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A138" s="16"/>
-      <c r="B138" s="16"/>
-      <c r="C138" s="16"/>
-      <c r="D138" s="16"/>
-      <c r="E138" s="16"/>
-      <c r="F138" s="16"/>
-      <c r="G138" s="16"/>
-      <c r="H138" s="16"/>
-      <c r="I138" s="16"/>
-      <c r="J138" s="16"/>
-      <c r="K138" s="16"/>
+      <c r="C138" s="17"/>
+      <c r="D138" s="17"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="17"/>
+      <c r="G138" s="17"/>
+      <c r="H138" s="17"/>
+      <c r="I138" s="17"/>
+      <c r="J138" s="17"/>
+      <c r="K138" s="17"/>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A139" s="3" t="s">
+      <c r="A139" s="17"/>
+      <c r="B139" s="17"/>
+      <c r="C139" s="17"/>
+      <c r="D139" s="17"/>
+      <c r="E139" s="17"/>
+      <c r="F139" s="17"/>
+      <c r="G139" s="17"/>
+      <c r="H139" s="17"/>
+      <c r="I139" s="17"/>
+      <c r="J139" s="17"/>
+      <c r="K139" s="17"/>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B139" s="3" t="s">
+      <c r="B140" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C139" s="3" t="s">
+      <c r="C140" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D139" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E139" s="3" t="s">
+      <c r="D140" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E140" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F139" s="3" t="s">
+      <c r="F140" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G139" s="3" t="s">
+      <c r="G140" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H139" s="3" t="s">
+      <c r="H140" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I139" s="3" t="s">
+      <c r="I140" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J139" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K139" s="3" t="s">
+      <c r="J140" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K140" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B140" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C140" s="7">
-        <v>4</v>
-      </c>
-      <c r="D140" s="7">
-        <v>10</v>
-      </c>
-      <c r="E140" s="7">
-        <v>0</v>
-      </c>
-      <c r="F140" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G140" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H140" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I140" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J140" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K140" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C141" s="7">
+        <v>4</v>
+      </c>
+      <c r="D141" s="7">
+        <v>10</v>
+      </c>
+      <c r="E141" s="7">
+        <v>0</v>
+      </c>
+      <c r="F141" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G141" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H141" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I141" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J141" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K141" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B141" s="7" t="s">
+      <c r="B142" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C141" s="7">
+      <c r="C142" s="7">
         <v>200</v>
       </c>
-      <c r="D141" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E141" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F141" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G141" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H141" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I141" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J141" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K141" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A144" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B144" s="16" t="s">
+      <c r="D142" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F142" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G142" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H142" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I142" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J142" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K142" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A145" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B145" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C144" s="16"/>
-      <c r="D144" s="16"/>
-      <c r="E144" s="16"/>
-      <c r="F144" s="16"/>
-      <c r="G144" s="16"/>
-      <c r="H144" s="16"/>
-      <c r="I144" s="16"/>
-      <c r="J144" s="16"/>
-      <c r="K144" s="16"/>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A145" s="16"/>
-      <c r="B145" s="16"/>
-      <c r="C145" s="16"/>
-      <c r="D145" s="16"/>
-      <c r="E145" s="16"/>
-      <c r="F145" s="16"/>
-      <c r="G145" s="16"/>
-      <c r="H145" s="16"/>
-      <c r="I145" s="16"/>
-      <c r="J145" s="16"/>
-      <c r="K145" s="16"/>
+      <c r="C145" s="17"/>
+      <c r="D145" s="17"/>
+      <c r="E145" s="17"/>
+      <c r="F145" s="17"/>
+      <c r="G145" s="17"/>
+      <c r="H145" s="17"/>
+      <c r="I145" s="17"/>
+      <c r="J145" s="17"/>
+      <c r="K145" s="17"/>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A146" s="3" t="s">
+      <c r="A146" s="17"/>
+      <c r="B146" s="17"/>
+      <c r="C146" s="17"/>
+      <c r="D146" s="17"/>
+      <c r="E146" s="17"/>
+      <c r="F146" s="17"/>
+      <c r="G146" s="17"/>
+      <c r="H146" s="17"/>
+      <c r="I146" s="17"/>
+      <c r="J146" s="17"/>
+      <c r="K146" s="17"/>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B146" s="3" t="s">
+      <c r="B147" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C146" s="3" t="s">
+      <c r="C147" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D146" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E146" s="3" t="s">
+      <c r="D147" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E147" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F146" s="3" t="s">
+      <c r="F147" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G146" s="3" t="s">
+      <c r="G147" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H146" s="3" t="s">
+      <c r="H147" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I146" s="3" t="s">
+      <c r="I147" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J146" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K146" s="3" t="s">
+      <c r="J147" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K147" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A147" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B147" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C147" s="7">
-        <v>4</v>
-      </c>
-      <c r="D147" s="7">
-        <v>10</v>
-      </c>
-      <c r="E147" s="7">
-        <v>0</v>
-      </c>
-      <c r="F147" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G147" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H147" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I147" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J147" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K147" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B148" s="7" t="s">
         <v>15</v>
@@ -4123,10 +4123,10 @@
       <c r="C148" s="7">
         <v>4</v>
       </c>
-      <c r="D148" s="3">
-        <v>10</v>
-      </c>
-      <c r="E148" s="3">
+      <c r="D148" s="7">
+        <v>10</v>
+      </c>
+      <c r="E148" s="7">
         <v>0</v>
       </c>
       <c r="F148" s="7" t="s">
@@ -4142,7 +4142,7 @@
         <v>19</v>
       </c>
       <c r="J148" s="3" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="K148" s="3" t="s">
         <v>18</v>
@@ -4150,34 +4150,34 @@
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C149" s="7">
-        <v>10</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>18</v>
+        <v>4</v>
+      </c>
+      <c r="D149" s="3">
+        <v>10</v>
+      </c>
+      <c r="E149" s="3">
+        <v>0</v>
       </c>
       <c r="F149" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G149" s="7" t="s">
-        <v>19</v>
+      <c r="G149" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="H149" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I149" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J149" s="3" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="K149" s="3" t="s">
         <v>18</v>
@@ -4185,13 +4185,13 @@
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="B150" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C150" s="7">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>18</v>
@@ -4199,8 +4199,8 @@
       <c r="E150" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F150" s="15" t="s">
-        <v>20</v>
+      <c r="F150" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="G150" s="7" t="s">
         <v>19</v>
@@ -4220,7 +4220,7 @@
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B151" s="7" t="s">
         <v>16</v>
@@ -4253,40 +4253,75 @@
         <v>18</v>
       </c>
     </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C152" s="7">
+        <v>100</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F152" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G152" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H152" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I152" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J152" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K152" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A144:A145"/>
-    <mergeCell ref="B144:K145"/>
-    <mergeCell ref="A119:A120"/>
-    <mergeCell ref="B119:K120"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="B129:K130"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="B137:K138"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:K93"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="B102:K103"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="B109:K110"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:K3"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:K11"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:K21"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:K41"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:K48"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:K56"/>
     <mergeCell ref="A63:A64"/>
     <mergeCell ref="B63:K64"/>
     <mergeCell ref="A74:A75"/>
     <mergeCell ref="B74:K75"/>
     <mergeCell ref="A83:A84"/>
     <mergeCell ref="B83:K84"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:K41"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:K48"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:K56"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:K3"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:K11"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:K21"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="B93:K94"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="B103:K104"/>
+    <mergeCell ref="A110:A111"/>
+    <mergeCell ref="B110:K111"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="B145:K146"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="B120:K121"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="B130:K131"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="B138:K139"/>
   </mergeCells>
   <conditionalFormatting sqref="J79:K79">
     <cfRule type="uniqueValues" dxfId="1" priority="2"/>

</xml_diff>